<commit_message>
memmap implementation does not work here
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,52 +461,32 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ST_fitting_time</t>
+          <t>Fit time STDT</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>ST_prediction_time</t>
+          <t>Prediction time STDT</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>SIM_fitting_time</t>
+          <t>Score STDT</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>SIM_prediction_time</t>
+          <t>Fit time CondensedDT</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>st_depth</t>
+          <t>Prediction time CondensedDT</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>st_nodes</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>sim_depth</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>sim_nodes</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>ST_score</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>SIM_score</t>
+          <t>Score CondensedDT</t>
         </is>
       </c>
     </row>
@@ -531,34 +511,22 @@
         <v>8</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01699924468994141</v>
+        <v>0.01599884033203125</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.01701259613037109</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.007521390914916992</v>
+        <v>0.02599978446960449</v>
       </c>
       <c r="J2" t="n">
-        <v>7</v>
+        <v>0.003999948501586914</v>
       </c>
       <c r="K2" t="n">
-        <v>19</v>
-      </c>
-      <c r="L2" t="n">
-        <v>8</v>
-      </c>
-      <c r="M2" t="n">
-        <v>29</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3">
@@ -582,34 +550,22 @@
         <v>8</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1365194320678711</v>
+        <v>0.1229982376098633</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03399991989135742</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="I3" t="n">
-        <v>0.02953100204467773</v>
+        <v>0.04700374603271484</v>
       </c>
       <c r="J3" t="n">
-        <v>5</v>
+        <v>0.01999711990356445</v>
       </c>
       <c r="K3" t="n">
-        <v>13</v>
-      </c>
-      <c r="L3" t="n">
-        <v>9</v>
-      </c>
-      <c r="M3" t="n">
-        <v>69</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.9166666666666666</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.3055555555555556</v>
       </c>
     </row>
     <row r="4">
@@ -633,34 +589,22 @@
         <v>8</v>
       </c>
       <c r="F4" t="n">
-        <v>2.388534545898438</v>
+        <v>2.365621328353882</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1670000553131104</v>
+        <v>0.9298245614035088</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2420001029968262</v>
+        <v>0.1370000839233398</v>
       </c>
       <c r="J4" t="n">
-        <v>8</v>
+        <v>0.1309998035430908</v>
       </c>
       <c r="K4" t="n">
-        <v>31</v>
-      </c>
-      <c r="L4" t="n">
-        <v>9</v>
-      </c>
-      <c r="M4" t="n">
-        <v>83</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.9298245614035088</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.8771929824561403</v>
+        <v>0.5526315789473685</v>
       </c>
     </row>
     <row r="5">
@@ -684,34 +628,22 @@
         <v>8</v>
       </c>
       <c r="F5" t="n">
-        <v>1.33398699760437</v>
+        <v>1.332000017166138</v>
       </c>
       <c r="G5" t="n">
-        <v>0.001000642776489258</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>3.376995086669922</v>
+        <v>0.8694444444444445</v>
       </c>
       <c r="I5" t="n">
-        <v>1.918703556060791</v>
+        <v>1.445001840591431</v>
       </c>
       <c r="J5" t="n">
-        <v>9</v>
+        <v>1.197999477386475</v>
       </c>
       <c r="K5" t="n">
-        <v>153</v>
-      </c>
-      <c r="L5" t="n">
-        <v>9</v>
-      </c>
-      <c r="M5" t="n">
-        <v>189</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.8694444444444445</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.675</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglant gower distance again
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -496,13 +496,13 @@
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01300048828125</v>
+        <v>0.0157010555267334</v>
       </c>
       <c r="G2" t="n">
-        <v>0.009001016616821289</v>
+        <v>0.001296758651733398</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -526,13 +526,13 @@
         <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0149986743927002</v>
+        <v>0.02471041679382324</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01300454139709473</v>
+        <v>0.004382848739624023</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>0.9444444444444444</v>
       </c>
     </row>
     <row r="4">
@@ -556,13 +556,13 @@
         <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>0.06099796295166016</v>
+        <v>0.0504612922668457</v>
       </c>
       <c r="G4" t="n">
-        <v>0.04999971389770508</v>
+        <v>0.01475977897644043</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8947368421052632</v>
+        <v>0.9210526315789473</v>
       </c>
     </row>
     <row r="5">
@@ -586,13 +586,13 @@
         <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>0.44700026512146</v>
+        <v>0.1928677558898926</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3879988193511963</v>
+        <v>0.09611129760742188</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7055555555555556</v>
+        <v>0.7444444444444445</v>
       </c>
     </row>
     <row r="6">
@@ -616,13 +616,13 @@
         <v>10</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0370025634765625</v>
+        <v>0.1171343326568604</v>
       </c>
       <c r="G6" t="n">
-        <v>0.02699995040893555</v>
+        <v>0.03694820404052734</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9818181818181818</v>
+        <v>0.9963636363636363</v>
       </c>
     </row>
     <row r="7">
@@ -646,13 +646,13 @@
         <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>2.203777313232422</v>
+        <v>3.9241783618927</v>
       </c>
       <c r="G7" t="n">
-        <v>1.125008106231689</v>
+        <v>0.3028881549835205</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8975557153127247</v>
+        <v>0.8889288281811646</v>
       </c>
     </row>
     <row r="8">
@@ -676,13 +676,13 @@
         <v>10</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8090870380401611</v>
+        <v>1.786609172821045</v>
       </c>
       <c r="G8" t="n">
-        <v>0.06500935554504395</v>
+        <v>0.06383275985717773</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9910344827586207</v>
+        <v>0.9894827586206897</v>
       </c>
     </row>
     <row r="9">
@@ -706,13 +706,13 @@
         <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>1.243401765823364</v>
+        <v>2.114028215408325</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4274885654449463</v>
+        <v>0.397730827331543</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8135940219060293</v>
+        <v>0.8212713686150066</v>
       </c>
     </row>
     <row r="10">
@@ -736,13 +736,13 @@
         <v>10</v>
       </c>
       <c r="F10" t="n">
-        <v>14.1006190776825</v>
+        <v>19.88306164741516</v>
       </c>
       <c r="G10" t="n">
-        <v>4.163985252380371</v>
+        <v>6.864698886871338</v>
       </c>
       <c r="H10" t="n">
-        <v>0.865175</v>
+        <v>0.877365</v>
       </c>
     </row>
     <row r="11">
@@ -766,13 +766,13 @@
         <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>0.334000825881958</v>
+        <v>0.1742157936096191</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1289989948272705</v>
+        <v>0.04530668258666992</v>
       </c>
       <c r="H11" t="n">
-        <v>7165.820224719101</v>
+        <v>7697.213483146067</v>
       </c>
     </row>
     <row r="12">
@@ -796,13 +796,13 @@
         <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3909981250762939</v>
+        <v>0.2116374969482422</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1669998168945312</v>
+        <v>0.0632331371307373</v>
       </c>
       <c r="H12" t="n">
-        <v>1702.039215686274</v>
+        <v>1783.098039215686</v>
       </c>
     </row>
     <row r="13">
@@ -826,13 +826,13 @@
         <v>10</v>
       </c>
       <c r="F13" t="n">
-        <v>0.8839554786682129</v>
+        <v>0.2446317672729492</v>
       </c>
       <c r="G13" t="n">
-        <v>0.3900136947631836</v>
+        <v>0.1688055992126465</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9336542364384689</v>
+        <v>0.9080902635702518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor Gower similarity calculation with Numba optimization
- Added a new implementation of the Gower similarity function in `myGower.py` using Numba for performance improvements.
- Removed commented-out legacy code for clarity.
- Introduced efficient handling of numerical and categorical features using masks.
- Updated the similarity calculation to return a combined score based on both numerical and categorical differences.
- Generated new compiled files for `SimilarityDecisionTree_D11` and `MeanSimilarityDTClassifier_D8` to reflect the latest changes.
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,17 +461,17 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Fit time SDTree_D10</t>
+          <t>Fit time DSTree_D10</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Prediction time SDTree_D10</t>
+          <t>Prediction time DSTree_D10</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Score SDTree_D10</t>
+          <t>Score DSTree_D10</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -511,19 +511,19 @@
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>0.002999544143676758</v>
+        <v>0.007318735122680664</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00100255012512207</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="I2" t="n">
-        <v>0.003000020980834961</v>
+        <v>6.34464955329895</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>0.002009868621826172</v>
       </c>
       <c r="K2" t="n">
         <v>0.9</v>
@@ -550,22 +550,22 @@
         <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>0.005000829696655273</v>
+        <v>0.01031112670898438</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0009989738464355469</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>0.8888888888888888</v>
       </c>
       <c r="I3" t="n">
-        <v>0.004001379013061523</v>
+        <v>0.007329702377319336</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0009968280792236328</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8611111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
     </row>
     <row r="4">
@@ -589,19 +589,19 @@
         <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>0.009999275207519531</v>
+        <v>0.03126907348632812</v>
       </c>
       <c r="G4" t="n">
-        <v>0.003999948501586914</v>
+        <v>0.002786636352539062</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9210526315789473</v>
+        <v>0.9298245614035088</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01300263404846191</v>
+        <v>0.01590800285339355</v>
       </c>
       <c r="J4" t="n">
-        <v>0.003998041152954102</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
         <v>0.9473684210526315</v>
@@ -628,22 +628,22 @@
         <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>0.07700324058532715</v>
+        <v>0.1158242225646973</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01899623870849609</v>
+        <v>0.03172445297241211</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7055555555555556</v>
+        <v>0.7027777777777777</v>
       </c>
       <c r="I5" t="n">
-        <v>0.07200002670288086</v>
+        <v>0.09540414810180664</v>
       </c>
       <c r="J5" t="n">
-        <v>0.01699995994567871</v>
+        <v>0.01597309112548828</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7444444444444445</v>
+        <v>0.6722222222222223</v>
       </c>
     </row>
     <row r="6">
@@ -667,22 +667,22 @@
         <v>10</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01400017738342285</v>
+        <v>0.02765989303588867</v>
       </c>
       <c r="G6" t="n">
-        <v>0.004999876022338867</v>
+        <v>0.007353782653808594</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9381818181818182</v>
+        <v>0.92</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01400041580200195</v>
+        <v>0.02443718910217285</v>
       </c>
       <c r="J6" t="n">
-        <v>0.004999876022338867</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9345454545454546</v>
+        <v>0.9490909090909091</v>
       </c>
     </row>
     <row r="7">
@@ -706,22 +706,22 @@
         <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>1.653957366943359</v>
+        <v>2.404195785522461</v>
       </c>
       <c r="G7" t="n">
-        <v>0.06301283836364746</v>
+        <v>0.1112713813781738</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8921639108554996</v>
+        <v>0.8914450035945363</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3553156852722168</v>
+        <v>7.670363426208496</v>
       </c>
       <c r="J7" t="n">
-        <v>0.06101608276367188</v>
+        <v>4.025373458862305</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8989935298346513</v>
+        <v>0.8914450035945363</v>
       </c>
     </row>
     <row r="8">
@@ -745,217 +745,22 @@
         <v>10</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7932195663452148</v>
+        <v>0.350999116897583</v>
       </c>
       <c r="G8" t="n">
-        <v>0.02351546287536621</v>
+        <v>0.04653596878051758</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9906896551724138</v>
+        <v>0.9906034482758621</v>
       </c>
       <c r="I8" t="n">
-        <v>0.200228214263916</v>
+        <v>4.064779996871948</v>
       </c>
       <c r="J8" t="n">
-        <v>0.01700592041015625</v>
+        <v>0.01574206352233887</v>
       </c>
       <c r="K8" t="n">
-        <v>0.9907758620689655</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Adult</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>48842</v>
-      </c>
-      <c r="D9" t="n">
-        <v>14</v>
-      </c>
-      <c r="E9" t="n">
-        <v>10</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1.122697830200195</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.177009105682373</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.8066332275565564</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.5317456722259521</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.159027099609375</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.8190193469137066</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Hepatitis</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="D10" t="n">
-        <v>19</v>
-      </c>
-      <c r="E10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F10" t="n">
-        <v>12.9577317237854</v>
-      </c>
-      <c r="G10" t="n">
-        <v>3.523000240325928</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.86436</v>
-      </c>
-      <c r="I10" t="n">
-        <v>12.71368479728699</v>
-      </c>
-      <c r="J10" t="n">
-        <v>3.504999876022339</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.87135</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Diabetes Progression</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>regression</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>442</v>
-      </c>
-      <c r="D11" t="n">
-        <v>10</v>
-      </c>
-      <c r="E11" t="n">
-        <v>10</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.02099919319152832</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.004998445510864258</v>
-      </c>
-      <c r="H11" t="n">
-        <v>4088.47191011236</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.01999998092651367</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.00500035285949707</v>
-      </c>
-      <c r="K11" t="n">
-        <v>4641.752808988764</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Boston Housing</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>regression</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>506</v>
-      </c>
-      <c r="D12" t="n">
-        <v>13</v>
-      </c>
-      <c r="E12" t="n">
-        <v>10</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.02900099754333496</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.006998300552368164</v>
-      </c>
-      <c r="H12" t="n">
-        <v>1888.558823529412</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.0279998779296875</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.006000041961669922</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1590.088235294118</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>California Housing</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>regression</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>20640</v>
-      </c>
-      <c r="D13" t="n">
-        <v>8</v>
-      </c>
-      <c r="E13" t="n">
-        <v>10</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.0988311767578125</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.06201386451721191</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.9254657965159883</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.1410000324249268</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.05599713325500488</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.925583533919089</v>
+        <v>0.9925862068965517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>